<commit_message>
Os ajustes solicitados em reunião de apresentação foram concluídos. Sujestão de melhoria na execução das validações na função upload que ficou um pouco demorado
</commit_message>
<xml_diff>
--- a/wcm/widget/cadastro_materiais_estoque/src/main/webapp/resources/images/padrao_upload_materiais.xlsx
+++ b/wcm/widget/cadastro_materiais_estoque/src/main/webapp/resources/images/padrao_upload_materiais.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CLEITONFERREIRADEPAU\OneDrive_ComBio\Documentos\projetos_fluig\solicitacao_de_compra_naormal_urgente\process_materiais_estoque\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D80C9206-9F9A-473A-A894-45AC65DED429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE6EDD8-2EDE-44E2-80E5-7A24BB8F7A9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21852" yWindow="924" windowWidth="21600" windowHeight="11292" xr2:uid="{23D15041-1C68-4325-81EB-6F98E9AC12C4}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{23D15041-1C68-4325-81EB-6F98E9AC12C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>DESCRIÇÃO</t>
   </si>
@@ -44,17 +44,23 @@
     <t>QUANTIDADE</t>
   </si>
   <si>
-    <t>COD_ESTAB</t>
-  </si>
-  <si>
-    <t>COD_ITEM</t>
+    <t>CÓDIGO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITEM </t>
+  </si>
+  <si>
+    <t>LOCALIZAÇÃO</t>
+  </si>
+  <si>
+    <t>COD_ESTABELECIMENTO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -62,21 +68,50 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -85,7 +120,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -422,32 +457,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{861A69AC-6A41-4260-B884-3661A7E7F069}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" customWidth="1"/>
+    <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>